<commit_message>
a lot of changes done for sonarqube
</commit_message>
<xml_diff>
--- a/backend/slack-hrbp/reports/Attendance_U08EMGH3ZUK_from_Mar-2025_to_Mar-2025.xlsx
+++ b/backend/slack-hrbp/reports/Attendance_U08EMGH3ZUK_from_Mar-2025_to_Mar-2025.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>Mar-2025 (Leave Date)</t>
   </si>
@@ -23,112 +23,115 @@
     <t>2025-03-01</t>
   </si>
   <si>
+    <t>Planned Leave</t>
+  </si>
+  <si>
+    <t>2025-03-02</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>2025-03-02</t>
-  </si>
-  <si>
     <t>2025-03-03</t>
   </si>
   <si>
+    <t>2025-03-04</t>
+  </si>
+  <si>
+    <t>2025-03-05</t>
+  </si>
+  <si>
+    <t>2025-03-06</t>
+  </si>
+  <si>
+    <t>2025-03-07</t>
+  </si>
+  <si>
+    <t>2025-03-08</t>
+  </si>
+  <si>
+    <t>2025-03-09</t>
+  </si>
+  <si>
+    <t>2025-03-10</t>
+  </si>
+  <si>
+    <t>2025-03-11</t>
+  </si>
+  <si>
+    <t>2025-03-12</t>
+  </si>
+  <si>
+    <t>2025-03-13</t>
+  </si>
+  <si>
+    <t>2025-03-14</t>
+  </si>
+  <si>
+    <t>2025-03-15</t>
+  </si>
+  <si>
+    <t>2025-03-16</t>
+  </si>
+  <si>
+    <t>2025-03-17</t>
+  </si>
+  <si>
+    <t>2025-03-18</t>
+  </si>
+  <si>
+    <t>2025-03-19</t>
+  </si>
+  <si>
+    <t>2025-03-20</t>
+  </si>
+  <si>
+    <t>2025-03-21</t>
+  </si>
+  <si>
+    <t>2025-03-22</t>
+  </si>
+  <si>
+    <t>2025-03-23</t>
+  </si>
+  <si>
+    <t>2025-03-24</t>
+  </si>
+  <si>
+    <t>2025-03-25</t>
+  </si>
+  <si>
+    <t>Unplanned Leave</t>
+  </si>
+  <si>
+    <t>2025-03-26</t>
+  </si>
+  <si>
+    <t>2025-03-27</t>
+  </si>
+  <si>
+    <t>2025-03-28</t>
+  </si>
+  <si>
+    <t>Travelling to HQ</t>
+  </si>
+  <si>
+    <t>2025-03-29</t>
+  </si>
+  <si>
+    <t>2025-03-30</t>
+  </si>
+  <si>
+    <t>2025-03-31</t>
+  </si>
+  <si>
+    <t>Mar-2025 Leave Summary</t>
+  </si>
+  <si>
     <t>Sick Leave</t>
   </si>
   <si>
-    <t>2025-03-04</t>
-  </si>
-  <si>
-    <t>2025-03-05</t>
-  </si>
-  <si>
-    <t>2025-03-06</t>
-  </si>
-  <si>
-    <t>2025-03-07</t>
-  </si>
-  <si>
-    <t>2025-03-08</t>
-  </si>
-  <si>
-    <t>2025-03-09</t>
-  </si>
-  <si>
-    <t>2025-03-10</t>
-  </si>
-  <si>
-    <t>Planned Leave</t>
-  </si>
-  <si>
-    <t>2025-03-11</t>
-  </si>
-  <si>
-    <t>2025-03-12</t>
-  </si>
-  <si>
-    <t>2025-03-13</t>
-  </si>
-  <si>
-    <t>2025-03-14</t>
-  </si>
-  <si>
-    <t>2025-03-15</t>
-  </si>
-  <si>
-    <t>2025-03-16</t>
-  </si>
-  <si>
-    <t>2025-03-17</t>
-  </si>
-  <si>
     <t>WFH</t>
-  </si>
-  <si>
-    <t>2025-03-18</t>
-  </si>
-  <si>
-    <t>2025-03-19</t>
-  </si>
-  <si>
-    <t>2025-03-20</t>
-  </si>
-  <si>
-    <t>Unplanned Leave</t>
-  </si>
-  <si>
-    <t>2025-03-21</t>
-  </si>
-  <si>
-    <t>2025-03-22</t>
-  </si>
-  <si>
-    <t>2025-03-23</t>
-  </si>
-  <si>
-    <t>2025-03-24</t>
-  </si>
-  <si>
-    <t>2025-03-25</t>
-  </si>
-  <si>
-    <t>2025-03-26</t>
-  </si>
-  <si>
-    <t>2025-03-27</t>
-  </si>
-  <si>
-    <t>2025-03-28</t>
-  </si>
-  <si>
-    <t>2025-03-29</t>
-  </si>
-  <si>
-    <t>2025-03-30</t>
-  </si>
-  <si>
-    <t>2025-03-31</t>
-  </si>
-  <si>
-    <t>Mar-2025 Leave Summary</t>
   </si>
 </sst>
 </file>
@@ -204,15 +207,15 @@
         <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -220,7 +223,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -228,7 +231,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7">
@@ -236,7 +239,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -244,7 +247,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -252,7 +255,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -260,7 +263,7 @@
         <v>12</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -268,108 +271,108 @@
         <v>13</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="0">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="0">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>22</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s" s="0">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s" s="0">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s" s="0">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="0">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s" s="0">
         <v>3</v>
@@ -377,103 +380,103 @@
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>14</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>3</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>26</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B36" t="n" s="0">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s" s="0">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B37" t="n" s="0">
-        <v>6.0</v>
+        <v>4.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B38" t="n" s="0">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s" s="0">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="B39" t="n" s="0">
-        <v>2.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>